<commit_message>
Add odd files for history
</commit_message>
<xml_diff>
--- a/team_rating.xlsx
+++ b/team_rating.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7DF834-14A6-4D0D-8AE7-6AB77EC351CE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56FDBDE-D36E-43F2-BF9B-984043A54FD2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Team Elo History" sheetId="6" r:id="rId3"/>
-    <sheet name="Team Active Elo 2010" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
+    <sheet name="Team Active Elo 2011" sheetId="8" r:id="rId4"/>
+    <sheet name="Team Active Elo 2010" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="314">
   <si>
     <t>EU</t>
   </si>
@@ -922,12 +923,6 @@
     <t>Current Elo</t>
   </si>
   <si>
-    <t>2010-09</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>SK Gaming</t>
   </si>
   <si>
@@ -940,31 +935,40 @@
     <t>AnotherStory</t>
   </si>
   <si>
-    <t>Fureur</t>
-  </si>
-  <si>
-    <t>Knight of Knowledge</t>
-  </si>
-  <si>
-    <t>Itkuvirsi</t>
-  </si>
-  <si>
-    <t>One Night Only</t>
-  </si>
-  <si>
-    <t>HUR DUR</t>
-  </si>
-  <si>
-    <t>TBA soon !</t>
-  </si>
-  <si>
-    <t>Toujours Devant</t>
-  </si>
-  <si>
-    <t>Polish Allstars</t>
-  </si>
-  <si>
     <t>2010-12</t>
+  </si>
+  <si>
+    <t>myRevenge</t>
+  </si>
+  <si>
+    <t>Team Dignitas</t>
+  </si>
+  <si>
+    <t>v8 eSports</t>
+  </si>
+  <si>
+    <t>RFLX Gaming</t>
+  </si>
+  <si>
+    <t>APictureOfAGoose</t>
+  </si>
+  <si>
+    <t>Chicks Dig Elo</t>
+  </si>
+  <si>
+    <t>NaJin e-mFire</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>For The Win</t>
+  </si>
+  <si>
+    <t>Team Jantelaget</t>
+  </si>
+  <si>
+    <t>Sex is our Life</t>
   </si>
 </sst>
 </file>
@@ -994,7 +998,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1031,11 +1035,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1065,11 +1104,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1395,8 +1488,8 @@
   <dimension ref="A1:AX413"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G319" sqref="G319"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A207" activeCellId="7" sqref="A184 A185 A186 A187 A198 A200 A206 A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4826,10 +4919,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976BBB26-CDEC-4C0E-8ACC-AE5ED3B52812}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4839,265 +4932,693 @@
     <col min="3" max="3" width="10" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="13">
+        <v>-62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="D1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="13">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="C2" s="9">
-        <v>-33</v>
-      </c>
-      <c r="D2" s="2">
-        <v>-33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>-21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>-8</v>
-      </c>
+      <c r="B5" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="13">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>-24</v>
-      </c>
+      <c r="A17" s="7"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="9">
-        <v>18</v>
-      </c>
-      <c r="D18" s="2">
-        <v>87</v>
-      </c>
+      <c r="A18" s="8"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2">
-        <v>-8</v>
-      </c>
+      <c r="A19" s="6"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>310</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>-24</v>
-      </c>
+      <c r="A20" s="6"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>33</v>
-      </c>
+      <c r="C21" s="18"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2">
-        <v>-24</v>
-      </c>
+      <c r="C22" s="18"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="C27" s="9">
-        <v>36</v>
-      </c>
-      <c r="D27" s="2">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="9">
-        <v>-21</v>
-      </c>
-      <c r="D28" s="2">
-        <v>-21</v>
-      </c>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A2 A6:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  <conditionalFormatting sqref="A1:A27 A29 A64:A1048576">
+    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23:A27">
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A29 A64:A1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E41F2C-697E-4ED3-A21F-A3D6C0F24AF1}">
+  <dimension ref="A1:C97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="13">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="9"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="9"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="13"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="13"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="13"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="13"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="13"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="13"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="13"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="13"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="13"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="13"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="13"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="13"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="13"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="13"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1 A67 A69:A1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:A1048576 A1">
+    <cfRule type="duplicateValues" dxfId="2" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A35">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A35">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B973AF-BF1B-4A13-B40B-E754847AD96E}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C20"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5118,212 +5639,47 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="13">
+        <v>-62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="13">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="B2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C2">
-        <v>-33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>-21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>310</v>
-      </c>
-      <c r="B16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" t="s">
-        <v>299</v>
-      </c>
-      <c r="C19">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="B20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20">
-        <v>-21</v>
+      <c r="B5" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="13">
+        <v>-25</v>
       </c>
     </row>
   </sheetData>
@@ -5331,7 +5687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3D3CC5-7823-4CA1-BF9B-C6B64BE9FBA8}">
   <dimension ref="A2:B3"/>
   <sheetViews>
@@ -5366,7 +5722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF77157-2C9C-4E09-A468-9E6565D4DE1C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -5430,7 +5786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E90DBC-AF7C-4372-B0CB-DD22E69739E0}">
   <dimension ref="A1:D38"/>
   <sheetViews>

</xml_diff>